<commit_message>
completare stat cu index, nume+prenume, contract.salariutarifar
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/downloads/Stat Salarii - Smecherie SRL - Septembrie 2020.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/downloads/Stat Salarii - Smecherie SRL - Septembrie 2020.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
   <si>
     <t xml:space="preserve">, </t>
   </si>
@@ -239,6 +239,27 @@
   </si>
   <si>
     <t>- Septembrie 2020 -</t>
+  </si>
+  <si>
+    <t>72 22</t>
+  </si>
+  <si>
+    <t>Date Personaleeee</t>
+  </si>
+  <si>
+    <t>Negoiță Bogdan-Ionuț</t>
+  </si>
+  <si>
+    <t>plis work</t>
+  </si>
+  <si>
+    <t>Pop Alexandru</t>
+  </si>
+  <si>
+    <t>Popescu Ion</t>
+  </si>
+  <si>
+    <t>Tataie Tataitzul</t>
   </si>
 </sst>
 </file>
@@ -246,7 +267,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
@@ -275,6 +296,17 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="7.0"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -823,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -856,7 +888,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -875,6 +906,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1201,7 +1236,7 @@
   <dimension ref="A1:V35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1210,7 +1245,7 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="14.28515625" collapsed="false"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="13.42578125" collapsed="false"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.7109375" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.28515625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.140625" collapsed="false"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="4.0" collapsed="false"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="4.28515625" collapsed="false"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="3.7109375" collapsed="false"/>
@@ -1230,49 +1265,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
     </row>
     <row r="4" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="L4" s="18" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="L4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
     </row>
     <row r="5" spans="1:21" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="L5" s="19" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="L5" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1343,21 +1378,21 @@
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22" t="s">
+      <c r="C9" s="20"/>
+      <c r="D9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="22"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="21"/>
       <c r="I9" s="9" t="s">
         <v>7</v>
       </c>
@@ -1435,14 +1470,14 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17" t="s">
+      <c r="C11" s="25"/>
+      <c r="D11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="17"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="8" t="s">
         <v>27</v>
       </c>
@@ -1494,10 +1529,10 @@
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="16"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -1547,10 +1582,10 @@
       <c r="I13" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="17"/>
+      <c r="K13" s="16"/>
       <c r="L13" s="8" t="s">
         <v>51</v>
       </c>
@@ -1616,11 +1651,17 @@
       <c r="U14" s="13"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="26"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="29" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>75</v>
+      </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
+      <c r="E15" s="26" t="n">
+        <v>21213.0</v>
+      </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
@@ -1636,10 +1677,10 @@
       <c r="R15" s="14"/>
       <c r="S15" s="14"/>
       <c r="T15" s="14"/>
-      <c r="U15" s="29"/>
+      <c r="U15" s="32"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="27"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -1659,56 +1700,62 @@
       <c r="R16" s="15"/>
       <c r="S16" s="15"/>
       <c r="T16" s="15"/>
-      <c r="U16" s="30"/>
+      <c r="U16" s="33"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A17" s="28"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="25"/>
-      <c r="U17" s="31"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="34"/>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="33"/>
-      <c r="T18" s="33"/>
-      <c r="U18" s="34"/>
+      <c r="A18" s="35" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="26" t="n">
+        <v>5000.0</v>
+      </c>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="37"/>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A19" s="27"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -1728,56 +1775,62 @@
       <c r="R19" s="15"/>
       <c r="S19" s="15"/>
       <c r="T19" s="15"/>
-      <c r="U19" s="30"/>
+      <c r="U19" s="33"/>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
-      <c r="S20" s="25"/>
-      <c r="T20" s="25"/>
-      <c r="U20" s="31"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="34"/>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="33"/>
-      <c r="S21" s="33"/>
-      <c r="T21" s="33"/>
-      <c r="U21" s="34"/>
+      <c r="A21" s="35" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="26" t="n">
+        <v>6154.0</v>
+      </c>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="36"/>
+      <c r="U21" s="37"/>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A22" s="27"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -1797,59 +1850,65 @@
       <c r="R22" s="15"/>
       <c r="S22" s="15"/>
       <c r="T22" s="15"/>
-      <c r="U22" s="30"/>
+      <c r="U22" s="33"/>
       <c r="V22" s="7"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A23" s="28"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="25"/>
-      <c r="T23" s="25"/>
-      <c r="U23" s="31"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="28"/>
+      <c r="S23" s="28"/>
+      <c r="T23" s="28"/>
+      <c r="U23" s="34"/>
       <c r="V23" s="7"/>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A24" s="32"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="33"/>
-      <c r="S24" s="33"/>
-      <c r="T24" s="33"/>
-      <c r="U24" s="34"/>
+      <c r="A24" s="35" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B24" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="26" t="n">
+        <v>2508.0</v>
+      </c>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="36"/>
+      <c r="R24" s="36"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="36"/>
+      <c r="U24" s="37"/>
       <c r="V24" s="7"/>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" s="27"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -1869,57 +1928,63 @@
       <c r="R25" s="15"/>
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
-      <c r="U25" s="30"/>
+      <c r="U25" s="33"/>
       <c r="V25" s="7"/>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A26" s="28"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
-      <c r="P26" s="25"/>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="25"/>
-      <c r="S26" s="25"/>
-      <c r="T26" s="25"/>
-      <c r="U26" s="31"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="28"/>
+      <c r="S26" s="28"/>
+      <c r="T26" s="28"/>
+      <c r="U26" s="34"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A27" s="32"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="33"/>
-      <c r="S27" s="33"/>
-      <c r="T27" s="33"/>
-      <c r="U27" s="34"/>
+      <c r="A27" s="35" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B27" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="26" t="n">
+        <v>6154.0</v>
+      </c>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="36"/>
+      <c r="N27" s="36"/>
+      <c r="O27" s="36"/>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="36"/>
+      <c r="R27" s="36"/>
+      <c r="S27" s="36"/>
+      <c r="T27" s="36"/>
+      <c r="U27" s="37"/>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A28" s="27"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
@@ -1939,56 +2004,62 @@
       <c r="R28" s="15"/>
       <c r="S28" s="15"/>
       <c r="T28" s="15"/>
-      <c r="U28" s="30"/>
+      <c r="U28" s="33"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A29" s="28"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="25"/>
-      <c r="S29" s="25"/>
-      <c r="T29" s="25"/>
-      <c r="U29" s="31"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
+      <c r="S29" s="28"/>
+      <c r="T29" s="28"/>
+      <c r="U29" s="34"/>
     </row>
     <row r="30" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="32"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="33"/>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
-      <c r="P30" s="33"/>
-      <c r="Q30" s="33"/>
-      <c r="R30" s="33"/>
-      <c r="S30" s="33"/>
-      <c r="T30" s="33"/>
-      <c r="U30" s="34"/>
+      <c r="A30" s="35" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="26" t="n">
+        <v>1197.0</v>
+      </c>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="36"/>
+      <c r="U30" s="37"/>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A31" s="27"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -2008,83 +2079,89 @@
       <c r="R31" s="7"/>
       <c r="S31" s="7"/>
       <c r="T31" s="7"/>
-      <c r="U31" s="30"/>
+      <c r="U31" s="33"/>
     </row>
     <row r="32">
-      <c r="A32" s="28"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
-      <c r="O32" s="25"/>
-      <c r="P32" s="25"/>
-      <c r="Q32" s="25"/>
-      <c r="R32" s="25"/>
-      <c r="S32" s="25"/>
-      <c r="T32" s="25"/>
-      <c r="U32" s="31"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="28"/>
+      <c r="S32" s="28"/>
+      <c r="T32" s="28"/>
+      <c r="U32" s="34"/>
     </row>
     <row r="33">
-      <c r="A33" s="32"/>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="33"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="33"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="33"/>
-      <c r="P33" s="33"/>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="33"/>
-      <c r="S33" s="33"/>
-      <c r="T33" s="33"/>
-      <c r="U33" s="34"/>
+      <c r="A33" s="35" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B33" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="26" t="n">
+        <v>21000.0</v>
+      </c>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="36"/>
+      <c r="T33" s="36"/>
+      <c r="U33" s="37"/>
     </row>
     <row r="34">
-      <c r="A34" s="27"/>
-      <c r="U34" s="30"/>
+      <c r="A34" s="30"/>
+      <c r="U34" s="33"/>
     </row>
     <row r="35">
-      <c r="A35" s="28"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="25"/>
-      <c r="P35" s="25"/>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="25"/>
-      <c r="S35" s="25"/>
-      <c r="T35" s="25"/>
-      <c r="U35" s="31"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="28"/>
+      <c r="N35" s="28"/>
+      <c r="O35" s="28"/>
+      <c r="P35" s="28"/>
+      <c r="Q35" s="28"/>
+      <c r="R35" s="28"/>
+      <c r="S35" s="28"/>
+      <c r="T35" s="28"/>
+      <c r="U35" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="21">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
@@ -2099,6 +2176,13 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="G9:H9"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B33:C33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>